<commit_message>
Patient Import Enhancements (#2564)
**Story card:** 

[ch3681](https://app.clubhouse.io/simpledotorg/story/3681/don-t-break-if-medical-history-question-is-blank)
[ch3680](https://app.clubhouse.io/simpledotorg/story/3680/support-y-n-m-f)
[ch3496](https://app.clubhouse.io/simpledotorg/story/3496/skip-rows-that-don-t-have-a-regn-date)

* Skip row if registration date is missing
* Don't break if diagnosis answers are missing
* Recognize gender abbreviations
* Recognize Y/N as Yes No for "Died?"
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/patient_import_invalid_data_test.xlsx
+++ b/spec/fixtures/files/patient_import_invalid_data_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharanmohanraj/code/simple/simple-server/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2567B80-A9BA-4145-B462-20763CD9BD4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C53EA9-C9BC-2744-AF0C-C6483E32A319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="134">
   <si>
     <t>registration_facility</t>
   </si>
@@ -428,6 +428,15 @@
   <si>
     <t>Vegetable District</t>
   </si>
+  <si>
+    <t>Random Gender</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>0000005</t>
+  </si>
 </sst>
 </file>
 
@@ -575,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -599,6 +608,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1524,23 +1536,81 @@
     </row>
     <row r="7" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
+      <c r="B7" s="23">
+        <v>44120.393055555556</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="12">
+        <v>67</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" s="12">
+        <v>936528787</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="T7" s="25">
+        <v>160</v>
+      </c>
+      <c r="U7" s="25">
+        <v>90</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="AA7" s="13"/>
       <c r="AB7" s="17"/>
       <c r="AC7" s="17"/>
@@ -1610,7 +1680,6 @@
       <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
@@ -15434,7 +15503,7 @@
           <x14:formula1>
             <xm:f>regions!$A$1:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N502</xm:sqref>
+          <xm:sqref>N3:N6 N8:N502</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
@@ -15446,7 +15515,7 @@
           <x14:formula1>
             <xm:f>'common medicines'!$A$1:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>U7:Z502 V3:Z6 AD3:AH502</xm:sqref>
+          <xm:sqref>AD3:AH502 V3:Z6 U8:Z502</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>